<commit_message>
Colorado water right update
Colorado water right update
</commit_message>
<xml_diff>
--- a/Colorado/WaterAllocation/CO_Allocation Schema Mapping_WaDEQA.xlsx
+++ b/Colorado/WaterAllocation/CO_Allocation Schema Mapping_WaDEQA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Colorado\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A352E1-1222-4EC5-91C8-FC0C6747C758}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE05C3C-08CE-4495-AD28-E81DC64842C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1692" windowWidth="23256" windowHeight="12576" tabRatio="700" activeTab="4" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="700" activeTab="6" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes and Reminders" sheetId="8" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="356">
   <si>
     <t>Name</t>
   </si>
@@ -1106,6 +1106,15 @@
   </si>
   <si>
     <t>fill blank spots with unspecified</t>
+  </si>
+  <si>
+    <t>OwnerClassificationCV</t>
+  </si>
+  <si>
+    <t>Army (USA)</t>
+  </si>
+  <si>
+    <t>WSWC defined owner tag.</t>
   </si>
 </sst>
 </file>
@@ -1983,7 +1992,7 @@
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2326,6 +2335,15 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -3832,7 +3850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC5F405-0A84-4CAE-BAB0-9DF044EAE9B9}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -4822,10 +4840,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B91B1FF-D207-4871-B787-27544A9D3030}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5778,7 +5796,7 @@
       </c>
       <c r="J32" s="97"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>98</v>
       </c>
@@ -5808,7 +5826,7 @@
       </c>
       <c r="J33" s="97"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>100</v>
       </c>
@@ -5838,7 +5856,7 @@
       </c>
       <c r="J34" s="97"/>
     </row>
-    <row r="35" spans="1:10" s="66" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" s="66" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="66" t="s">
         <v>162</v>
       </c>
@@ -5868,7 +5886,7 @@
       </c>
       <c r="J35" s="104"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>82</v>
       </c>
@@ -5898,7 +5916,7 @@
       </c>
       <c r="J36" s="99"/>
     </row>
-    <row r="37" spans="1:10" s="66" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" s="66" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="111" t="s">
         <v>342</v>
       </c>
@@ -5924,7 +5942,7 @@
       <c r="I37" s="113"/>
       <c r="J37" s="114"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>90</v>
       </c>
@@ -5954,7 +5972,7 @@
       </c>
       <c r="J38" s="97"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>91</v>
       </c>
@@ -5984,7 +6002,7 @@
       </c>
       <c r="J39" s="106"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>99</v>
       </c>
@@ -6014,7 +6032,7 @@
       </c>
       <c r="J40" s="97"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>96</v>
       </c>
@@ -6044,48 +6062,50 @@
       </c>
       <c r="J41" s="97"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" s="66" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>89</v>
+        <v>353</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D42" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E42" s="44" t="s">
-        <v>155</v>
-      </c>
-      <c r="F42" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="G42" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="H42" s="20" t="s">
+      <c r="D42" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="117"/>
+      <c r="H42" s="118" t="s">
         <v>38</v>
       </c>
       <c r="I42" s="97" t="s">
-        <v>38</v>
-      </c>
-      <c r="J42" s="97"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+      <c r="J42" s="119" t="s">
+        <v>355</v>
+      </c>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E43" s="44" t="s">
         <v>155</v>
@@ -6099,81 +6119,81 @@
       <c r="H43" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="I43" s="21" t="s">
+      <c r="I43" s="97" t="s">
+        <v>38</v>
+      </c>
+      <c r="J43" s="97"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E44" s="44" t="s">
+        <v>155</v>
+      </c>
+      <c r="F44" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="G44" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="H44" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="I44" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="J43" s="97"/>
-    </row>
-    <row r="44" spans="1:10" s="66" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="66" t="s">
+      <c r="J44" s="97"/>
+    </row>
+    <row r="45" spans="1:16" s="66" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="66" t="s">
         <v>156</v>
       </c>
-      <c r="B44" s="67" t="s">
+      <c r="B45" s="67" t="s">
         <v>105</v>
       </c>
-      <c r="C44" s="68" t="s">
+      <c r="C45" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="D44" s="70" t="s">
+      <c r="D45" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="E44" s="45" t="s">
+      <c r="E45" s="45" t="s">
         <v>133</v>
       </c>
-      <c r="F44" s="44"/>
-      <c r="G44" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="H44" s="96" t="s">
-        <v>38</v>
-      </c>
-      <c r="I44" s="45" t="s">
+      <c r="F45" s="44"/>
+      <c r="G45" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="H45" s="96" t="s">
+        <v>38</v>
+      </c>
+      <c r="I45" s="45" t="s">
         <v>133</v>
       </c>
-      <c r="J44" s="107"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" s="7" t="s">
+      <c r="J45" s="107"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B46" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E45" s="44" t="s">
-        <v>155</v>
-      </c>
-      <c r="F45" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="G45" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="H45" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="I45" s="97" t="s">
-        <v>38</v>
-      </c>
-      <c r="J45" s="97"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="E46" s="44" t="s">
         <v>155</v>
@@ -6187,10 +6207,40 @@
       <c r="H46" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="I46" s="21" t="s">
+      <c r="I46" s="97" t="s">
+        <v>38</v>
+      </c>
+      <c r="J46" s="97"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E47" s="44" t="s">
+        <v>155</v>
+      </c>
+      <c r="F47" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="G47" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="H47" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="I47" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="J46" s="97"/>
+      <c r="J47" s="97"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:J13">

</xml_diff>